<commit_message>
Update Protocol Team Noobcoder.xlsx
</commit_message>
<xml_diff>
--- a/Prototyping/Protocol Team Noobcoder.xlsx
+++ b/Prototyping/Protocol Team Noobcoder.xlsx
@@ -1,25 +1,99 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\HSHL\SOFTWARE FOR ELE\GitHub\Team Noobcoder\Prototyping\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F57D8154-3AA3-4386-A835-12EEFD4033EB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+  <si>
+    <t>Column1</t>
+  </si>
+  <si>
+    <t>Column2</t>
+  </si>
+  <si>
+    <t>Column3</t>
+  </si>
+  <si>
+    <t>Column4</t>
+  </si>
+  <si>
+    <t>Column5</t>
+  </si>
+  <si>
+    <t>Column6</t>
+  </si>
+  <si>
+    <t>Column7</t>
+  </si>
+  <si>
+    <t>Column8</t>
+  </si>
+  <si>
+    <t>Column9</t>
+  </si>
+  <si>
+    <t>Column10</t>
+  </si>
+  <si>
+    <t>Column11</t>
+  </si>
+  <si>
+    <t>Column12</t>
+  </si>
+  <si>
+    <t>Column13</t>
+  </si>
+  <si>
+    <t>Column14</t>
+  </si>
+  <si>
+    <t>Column15</t>
+  </si>
+  <si>
+    <t>Column16</t>
+  </si>
+  <si>
+    <t>Column17</t>
+  </si>
+  <si>
+    <t>Column18</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -49,13 +123,303 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="36">
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -66,6 +430,52 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{B8049470-5F36-4605-9951-F142EED26D8A}" name="Table3" displayName="Table3" ref="C3:T23" headerRowDxfId="18" dataDxfId="19">
+  <autoFilter ref="C3:T23" xr:uid="{B6739574-731A-462B-9DB6-BD771A9612BB}">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+    <filterColumn colId="4" hiddenButton="1"/>
+    <filterColumn colId="5" hiddenButton="1"/>
+    <filterColumn colId="6" hiddenButton="1"/>
+    <filterColumn colId="7" hiddenButton="1"/>
+    <filterColumn colId="8" hiddenButton="1"/>
+    <filterColumn colId="9" hiddenButton="1"/>
+    <filterColumn colId="10" hiddenButton="1"/>
+    <filterColumn colId="11" hiddenButton="1"/>
+    <filterColumn colId="12" hiddenButton="1"/>
+    <filterColumn colId="13" hiddenButton="1"/>
+    <filterColumn colId="14" hiddenButton="1"/>
+    <filterColumn colId="15" hiddenButton="1"/>
+    <filterColumn colId="16" hiddenButton="1"/>
+    <filterColumn colId="17" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="18">
+    <tableColumn id="1" xr3:uid="{44880A8D-B915-43B6-8CE3-91BE253A3E98}" name="Column1" totalsRowLabel="Total" dataDxfId="35" totalsRowDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{7FD2B959-9CB3-404E-A4BF-4B1169CFECFF}" name="Column2" dataDxfId="34" totalsRowDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{F84659BB-04F5-4AC3-AD6B-B529FA90E916}" name="Column3" dataDxfId="33" totalsRowDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{0E8D24BD-5CFB-4773-A643-2D3AE95DEDFA}" name="Column4" dataDxfId="32" totalsRowDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{FD9E558E-0017-48A5-B5EC-5B3C54239B4F}" name="Column5" dataDxfId="31" totalsRowDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{4F7B1B92-99BA-45F9-97E1-329C2B4D7447}" name="Column6" dataDxfId="30" totalsRowDxfId="7"/>
+    <tableColumn id="7" xr3:uid="{2A14BF04-2617-490C-871B-433484D4F39F}" name="Column7" dataDxfId="29" totalsRowDxfId="8"/>
+    <tableColumn id="8" xr3:uid="{A6DA931D-BD83-45B4-8C28-5E3D7186318B}" name="Column8" dataDxfId="28" totalsRowDxfId="9"/>
+    <tableColumn id="9" xr3:uid="{7B3F6AD0-2154-4BDF-BB43-D9CFC25EB908}" name="Column9" dataDxfId="27" totalsRowDxfId="10"/>
+    <tableColumn id="10" xr3:uid="{57931E3F-D675-4C74-AB07-596C88A70A82}" name="Column10" dataDxfId="26" totalsRowDxfId="11"/>
+    <tableColumn id="11" xr3:uid="{806EE126-3BC4-483F-B337-CEC0B33F674E}" name="Column11" dataDxfId="25" totalsRowDxfId="12"/>
+    <tableColumn id="12" xr3:uid="{0586F61E-322F-4149-8F8C-BBCE0A633DAD}" name="Column12" dataDxfId="24" totalsRowDxfId="13"/>
+    <tableColumn id="13" xr3:uid="{B93B4FB4-2DAC-48AE-A228-2B42C9C9CB90}" name="Column13" dataDxfId="23" totalsRowDxfId="14"/>
+    <tableColumn id="14" xr3:uid="{0FE9D500-678D-4F2D-B01F-1AEA2C06116B}" name="Column14" dataDxfId="22" totalsRowDxfId="15"/>
+    <tableColumn id="15" xr3:uid="{0A351855-00C4-453D-BF0A-7B409F0131B2}" name="Column15" dataDxfId="21" totalsRowDxfId="16"/>
+    <tableColumn id="16" xr3:uid="{58FE3FE2-BE69-4696-A015-B1004C931839}" name="Column16" dataDxfId="20" totalsRowDxfId="17"/>
+    <tableColumn id="17" xr3:uid="{9A555E12-5408-48A7-BC46-1D82A65E82CF}" name="Column17" totalsRowFunction="count"/>
+    <tableColumn id="18" xr3:uid="{8D0AEE2B-2EBC-4393-934D-109948E80D48}" name="Column18" dataDxfId="1" totalsRowDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium8" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -330,13 +740,444 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="C3:T23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="N5" sqref="N5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="10.5546875" customWidth="1"/>
+    <col min="4" max="11" width="10.44140625" customWidth="1"/>
+    <col min="12" max="19" width="11.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="3:20" x14ac:dyDescent="0.3">
+      <c r="C3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S3" t="s">
+        <v>16</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="3:20" x14ac:dyDescent="0.3">
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1"/>
+      <c r="T4" s="1"/>
+    </row>
+    <row r="5" spans="3:20" x14ac:dyDescent="0.3">
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="1"/>
+      <c r="T5" s="1"/>
+    </row>
+    <row r="6" spans="3:20" x14ac:dyDescent="0.3">
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="1"/>
+      <c r="T6" s="1"/>
+    </row>
+    <row r="7" spans="3:20" x14ac:dyDescent="0.3">
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="1"/>
+      <c r="T7" s="1"/>
+    </row>
+    <row r="8" spans="3:20" x14ac:dyDescent="0.3">
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="1"/>
+      <c r="T8" s="1"/>
+    </row>
+    <row r="9" spans="3:20" x14ac:dyDescent="0.3">
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1"/>
+      <c r="R9" s="1"/>
+      <c r="T9" s="1"/>
+    </row>
+    <row r="10" spans="3:20" x14ac:dyDescent="0.3">
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="1"/>
+      <c r="R10" s="1"/>
+      <c r="T10" s="1"/>
+    </row>
+    <row r="11" spans="3:20" x14ac:dyDescent="0.3">
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1"/>
+      <c r="R11" s="1"/>
+      <c r="T11" s="1"/>
+    </row>
+    <row r="12" spans="3:20" x14ac:dyDescent="0.3">
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+      <c r="Q12" s="1"/>
+      <c r="R12" s="1"/>
+      <c r="T12" s="1"/>
+    </row>
+    <row r="13" spans="3:20" x14ac:dyDescent="0.3">
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
+      <c r="Q13" s="1"/>
+      <c r="R13" s="1"/>
+      <c r="T13" s="1"/>
+    </row>
+    <row r="14" spans="3:20" x14ac:dyDescent="0.3">
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
+      <c r="Q14" s="1"/>
+      <c r="R14" s="1"/>
+      <c r="T14" s="1"/>
+    </row>
+    <row r="15" spans="3:20" x14ac:dyDescent="0.3">
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
+      <c r="Q15" s="1"/>
+      <c r="R15" s="1"/>
+      <c r="T15" s="1"/>
+    </row>
+    <row r="16" spans="3:20" x14ac:dyDescent="0.3">
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+      <c r="P16" s="1"/>
+      <c r="Q16" s="1"/>
+      <c r="R16" s="1"/>
+      <c r="T16" s="1"/>
+    </row>
+    <row r="17" spans="3:20" x14ac:dyDescent="0.3">
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+      <c r="P17" s="1"/>
+      <c r="Q17" s="1"/>
+      <c r="R17" s="1"/>
+      <c r="T17" s="1"/>
+    </row>
+    <row r="18" spans="3:20" x14ac:dyDescent="0.3">
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
+      <c r="M18" s="1"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+      <c r="P18" s="1"/>
+      <c r="Q18" s="1"/>
+      <c r="R18" s="1"/>
+      <c r="T18" s="1"/>
+    </row>
+    <row r="19" spans="3:20" x14ac:dyDescent="0.3">
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1"/>
+      <c r="M19" s="1"/>
+      <c r="N19" s="1"/>
+      <c r="O19" s="1"/>
+      <c r="P19" s="1"/>
+      <c r="Q19" s="1"/>
+      <c r="R19" s="1"/>
+      <c r="T19" s="1"/>
+    </row>
+    <row r="20" spans="3:20" x14ac:dyDescent="0.3">
+      <c r="T20" s="1"/>
+    </row>
+    <row r="21" spans="3:20" x14ac:dyDescent="0.3">
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="1"/>
+      <c r="M21" s="1"/>
+      <c r="N21" s="1"/>
+      <c r="O21" s="1"/>
+      <c r="P21" s="1"/>
+      <c r="Q21" s="1"/>
+      <c r="R21" s="1"/>
+      <c r="T21" s="1"/>
+    </row>
+    <row r="22" spans="3:20" x14ac:dyDescent="0.3">
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+      <c r="L22" s="1"/>
+      <c r="M22" s="1"/>
+      <c r="N22" s="1"/>
+      <c r="O22" s="1"/>
+      <c r="P22" s="1"/>
+      <c r="Q22" s="1"/>
+      <c r="R22" s="1"/>
+      <c r="T22" s="1"/>
+    </row>
+    <row r="23" spans="3:20" x14ac:dyDescent="0.3">
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="1"/>
+      <c r="M23" s="1"/>
+      <c r="N23" s="1"/>
+      <c r="O23" s="1"/>
+      <c r="P23" s="1"/>
+      <c r="Q23" s="1"/>
+      <c r="R23" s="1"/>
+      <c r="T23" s="1"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>